<commit_message>
Oppdatert prosjektplan, små oppdateringer på iterasjon
</commit_message>
<xml_diff>
--- a/MSF/Prosjektplan.xlsx
+++ b/MSF/Prosjektplan.xlsx
@@ -7,9 +7,9 @@
     <workbookView xWindow="140" yWindow="120" windowWidth="27840" windowHeight="15960" tabRatio="834"/>
   </bookViews>
   <sheets>
-    <sheet name="Eksempel_prosjektplan_MSF" sheetId="1" r:id="rId1"/>
+    <sheet name="Prosjektplan" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
   <si>
     <t>Beskrive brukerprofil</t>
   </si>
@@ -153,12 +153,6 @@
     <t>Omar Ilyas</t>
   </si>
   <si>
-    <t>Enighet om konsept byr på utfordringer</t>
-  </si>
-  <si>
-    <t>Samme som over</t>
-  </si>
-  <si>
     <t>Ikke startet</t>
   </si>
   <si>
@@ -168,31 +162,49 @@
     <t>Ferdig(for nå)</t>
   </si>
   <si>
-    <t>Usikkert hvem som trenger hva foreløpig</t>
-  </si>
-  <si>
-    <t>Ikke startet, testcase for alle forhold</t>
-  </si>
-  <si>
-    <t>Ikke ferdig, komponenter testes underveis.</t>
-  </si>
-  <si>
     <t>Ikke ferdig. Her regnes all dokumentasjon.</t>
   </si>
   <si>
     <t>Vurdert som ikke-relevant for dette prosjektet</t>
   </si>
   <si>
-    <t>Ikke startet, vurderes om relevant fortløpende.</t>
-  </si>
-  <si>
-    <t>ekstra tid lagt inn i tilfelle problemer oppstår</t>
-  </si>
-  <si>
-    <t>Ikke startet, nødvendighet vurderes fortløpende</t>
-  </si>
-  <si>
     <t>Ikke startet.</t>
+  </si>
+  <si>
+    <t>Fullført</t>
+  </si>
+  <si>
+    <t>Ikomponenter testes fortløpende.</t>
+  </si>
+  <si>
+    <t>Fullført, men valg av mer avansert teknologi lot tiden gå over estimert.</t>
+  </si>
+  <si>
+    <t>Dette punktet vil gå hånd i hånd med punktet under.</t>
+  </si>
+  <si>
+    <t>Brukers use cases som utgangspunkt for testing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alle har det de trenger tilgjengelig. </t>
+  </si>
+  <si>
+    <t>Ferdigstiller PHP/HTML/MySql</t>
+  </si>
+  <si>
+    <t>Ferdigstiller HTML/CSS</t>
+  </si>
+  <si>
+    <t>Ekstra tid lagt inn i tilfelle problemer oppstår.</t>
+  </si>
+  <si>
+    <t>Vurderes som ikke-relevant for dette prosjektet da det skal fremføres.</t>
+  </si>
+  <si>
+    <t>Brukerdokumentasjon legges under resultat av testing.</t>
+  </si>
+  <si>
+    <t>Fullført.</t>
   </si>
 </sst>
 </file>
@@ -646,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -658,7 +670,7 @@
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46" customWidth="1"/>
+    <col min="8" max="8" width="53.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27" customHeight="1">
@@ -712,14 +724,14 @@
         <v>2</v>
       </c>
       <c r="F5">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <f>E5-F5</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -773,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -800,7 +812,7 @@
         <v>-0.5</v>
       </c>
       <c r="H8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -820,14 +832,14 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -863,7 +875,7 @@
         <v>-1</v>
       </c>
       <c r="H12" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -890,7 +902,7 @@
         <v>-1.5</v>
       </c>
       <c r="H13" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -910,14 +922,14 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -944,7 +956,7 @@
         <v>0.5</v>
       </c>
       <c r="H15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -971,7 +983,7 @@
         <v>1.5</v>
       </c>
       <c r="H16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1000,14 +1012,14 @@
         <v>3</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1027,14 +1039,14 @@
         <v>3</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1054,14 +1066,14 @@
         <v>6</v>
       </c>
       <c r="F21">
-        <v>0.5</v>
+        <v>12</v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
-        <v>5.5</v>
+        <v>-6</v>
       </c>
       <c r="H21" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1081,14 +1093,14 @@
         <v>6</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G22">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="H22" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1142,7 +1154,7 @@
         <v>12</v>
       </c>
       <c r="H24" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1171,14 +1183,14 @@
         <v>6</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-4</v>
       </c>
       <c r="H27" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1198,14 +1210,14 @@
         <v>2</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="H28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1229,7 +1241,7 @@
         <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="24">
@@ -1246,17 +1258,17 @@
         <v>42466</v>
       </c>
       <c r="E30">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
       <c r="G30">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H30" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1282,17 +1294,17 @@
         <v>42467</v>
       </c>
       <c r="E33">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F33" s="17">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G33">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="H33" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1312,14 +1324,14 @@
         <v>4</v>
       </c>
       <c r="F34" s="17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G34">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H34" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1336,17 +1348,17 @@
         <v>42467</v>
       </c>
       <c r="E35">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F35" s="17">
         <v>0</v>
       </c>
       <c r="G35">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H35" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1366,14 +1378,14 @@
         <v>0.5</v>
       </c>
       <c r="F36" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="H36" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1393,14 +1405,14 @@
         <v>3</v>
       </c>
       <c r="F37" s="17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G37">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H37" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="13" thickBot="1">
@@ -1412,15 +1424,15 @@
       <c r="D38" s="4"/>
       <c r="E38" s="4">
         <f>SUM(E5:E37)</f>
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F38" s="4">
         <f>SUM(F5:F37)</f>
-        <v>33.1</v>
+        <v>92.1</v>
       </c>
       <c r="G38" s="4">
         <f>SUM(F5:F37)</f>
-        <v>33.1</v>
+        <v>92.1</v>
       </c>
       <c r="H38" s="4"/>
     </row>

</xml_diff>